<commit_message>
Next very rough draft without MetaEdOutput
</commit_message>
<xml_diff>
--- a/MetaEdOutput/MetaEd-Handbook.xlsx
+++ b/MetaEdOutput/MetaEd-Handbook.xlsx
@@ -13100,7 +13100,7 @@
         <x:v>ObservationType</x:v>
       </x:c>
       <x:c r="C222" s="2" t="str">
-        <x:v>The descriptor holds the previous career of an individual.</x:v>
+        <x:v>The descriptor holds the type (e.g., walkthrough, summative) of observation conducted.</x:v>
       </x:c>
       <x:c r="D222" s="2" t="str">
         <x:v>Descriptor</x:v>
@@ -13109,13 +13109,12 @@
         <x:v/>
       </x:c>
       <x:c r="F222" s="2" t="str">
-        <x:v>Accounting
-Consulting
-Education
-Maintenance
-Medical
+        <x:v>Formal
+Informal
 Other
-Science and Technology</x:v>
+Self Reflection
+Summative
+Walkthrough</x:v>
       </x:c>
       <x:c r="G222" s="2" t="str">
         <x:v/>
@@ -13123,7 +13122,7 @@
       <x:c r="H222" s="2" t="str">
         <x:v>&lt;xs:complexType name="EXTENSION-ObservationTypeDescriptor"&gt;
   &lt;xs:annotation&gt;
-    &lt;xs:documentation&gt;The descriptor holds the previous career of an individual.&lt;/xs:documentation&gt;
+    &lt;xs:documentation&gt;The descriptor holds the type (e.g., walkthrough, summative) of observation conducted.&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
       &lt;ann:TypeGroup&gt;Descriptor&lt;/ann:TypeGroup&gt;
     &lt;/xs:appinfo&gt;
@@ -29567,7 +29566,7 @@
         <x:v>ObservationTypeMap</x:v>
       </x:c>
       <x:c r="C410" s="2" t="str">
-        <x:v>Map for the type of previous careers.</x:v>
+        <x:v>Map for the observation types.</x:v>
       </x:c>
       <x:c r="D410" s="2" t="str">
         <x:v>Enumeration</x:v>
@@ -29576,13 +29575,12 @@
         <x:v/>
       </x:c>
       <x:c r="F410" s="2" t="str">
-        <x:v>Accounting
-Consulting
-Education
-Maintenance
-Medical
+        <x:v>Formal
+Informal
 Other
-Science and Technology</x:v>
+Self Reflection
+Summative
+Walkthrough</x:v>
       </x:c>
       <x:c r="G410" s="2" t="str">
         <x:v/>

</xml_diff>